<commit_message>
Updated work breakdown structure.
</commit_message>
<xml_diff>
--- a/scrum/Work breakdown structure.xlsx
+++ b/scrum/Work breakdown structure.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\Faculdade\3º Ano\1º Semestre\ES\jabref\scrum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Desktop\SE2122_57464_58763_57677_58125_63764\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD662076-3250-4509-BA21-F9467419216C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EB6F89-197B-41B1-927A-431CEA531BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{08C9D72D-549C-45FD-95B2-9CE6A514548F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{08C9D72D-549C-45FD-95B2-9CE6A514548F}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -51,16 +51,10 @@
     <t>Phase 1</t>
   </si>
   <si>
-    <t>Sprint1</t>
-  </si>
-  <si>
     <t>1.1.1</t>
   </si>
   <si>
     <t>Sprint Backlog</t>
-  </si>
-  <si>
-    <t>Burndown chart</t>
   </si>
   <si>
     <t>1.1.2</t>
@@ -140,6 +134,12 @@
   </si>
   <si>
     <t>To Do</t>
+  </si>
+  <si>
+    <t>Burndown Chart</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
   </si>
 </sst>
 </file>
@@ -250,28 +250,31 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Cor1" xfId="4" builtinId="31"/>
@@ -2255,169 +2258,169 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="10" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="6" width="10.88671875" customWidth="1"/>
+    <col min="7" max="10" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="3"/>
+    <row r="1" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="9"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="6"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B5" s="10" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8" t="s">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B7" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>7</v>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>11</v>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>14</v>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>16</v>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>18</v>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="8" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B14" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>24</v>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>25</v>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>26</v>
-      </c>
+    <row r="20" spans="16:20" x14ac:dyDescent="0.3">
+      <c r="T20" s="8"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="16:20" x14ac:dyDescent="0.25">
-      <c r="T20" s="10"/>
-    </row>
-    <row r="24" spans="16:20" x14ac:dyDescent="0.25">
-      <c r="P24" s="10"/>
+    <row r="24" spans="16:20" x14ac:dyDescent="0.3">
+      <c r="P24" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Finished first phase Work Breakdown Structure.
</commit_message>
<xml_diff>
--- a/scrum/Work breakdown structure.xlsx
+++ b/scrum/Work breakdown structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Desktop\SE2122_57464_58763_57677_58125_63764\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED7A5DA-E547-4CF1-9CD1-ECB3FEDC71C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD454A4-71C0-44BF-8CBE-6FF6D88AD08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{08C9D72D-549C-45FD-95B2-9CE6A514548F}"/>
   </bookViews>
@@ -250,7 +250,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -260,9 +260,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2258,7 +2255,7 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2271,10 +2268,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
@@ -2305,7 +2302,7 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2313,7 +2310,7 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2321,7 +2318,7 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2329,7 +2326,7 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2337,7 +2334,7 @@
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2345,7 +2342,7 @@
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2353,7 +2350,7 @@
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2361,7 +2358,7 @@
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2369,7 +2366,7 @@
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2377,7 +2374,7 @@
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2385,7 +2382,7 @@
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2393,7 +2390,7 @@
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2401,7 +2398,7 @@
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2409,7 +2406,7 @@
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>33</v>
       </c>
       <c r="C16" t="s">
@@ -2417,10 +2414,10 @@
       </c>
     </row>
     <row r="20" spans="16:20" x14ac:dyDescent="0.3">
-      <c r="T20" s="8"/>
+      <c r="T20" s="7"/>
     </row>
     <row r="24" spans="16:20" x14ac:dyDescent="0.3">
-      <c r="P24" s="8"/>
+      <c r="P24" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>